<commit_message>
Ko biết cmd gì
</commit_message>
<xml_diff>
--- a/WebTechnology/WebQuanLyBanHang/ExcelAddIn/bin/Debug/Book1.xlsx
+++ b/WebTechnology/WebQuanLyBanHang/ExcelAddIn/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re9ff915be6044cf3"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Ra3c0bdd6859a4c83"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5c1e3e089fa643ca"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rb79240681347406a"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{8b21d5f6-964d-4de0-b0ad-984182e1e865}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4f144214-7c38-4dbf-bc36-99e623609c96}">
   <we:reference id="c9f6dbb8-41b6-49a1-9d30-3797d2a32628" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
product detail and share
</commit_message>
<xml_diff>
--- a/WebTechnology/WebQuanLyBanHang/ExcelAddIn/bin/Debug/Book1.xlsx
+++ b/WebTechnology/WebQuanLyBanHang/ExcelAddIn/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R1d9266e5a6d743d3"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R02cf017094f44bb6"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R98b09418ad804996"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R30a18b8bf361411f"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{5d0ce161-32c2-44c7-a706-83e7449294db}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{dfda1139-60e7-438a-bdc9-c38fac61e88d}">
   <we:reference id="c9f6dbb8-41b6-49a1-9d30-3797d2a32628" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>